<commit_message>
change datum -> date
</commit_message>
<xml_diff>
--- a/Files/timeslots.xlsx
+++ b/Files/timeslots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bananenhoschi/Dev/fhnw/ip6/IP6-Optimal-Scheduling-of-Project-Presentations/Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\d\IP6-Optimal-Scheduling-of-Project-Presentations\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3157249-0E80-0F45-A812-2D21C70BB115}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3513313-F16B-4014-960F-427491EE0FF3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32720" yWindow="-1920" windowWidth="24740" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -25,30 +25,39 @@
     <author>tc={740B47BA-F5D4-4799-82B4-6217BAF24418}</author>
     <author>tc={99CDC6AA-F96E-4729-8D1D-2E4CD2479760}</author>
     <author>tc={BEA58940-8B8B-44F6-A1BC-72CF21AEA3A9}</author>
+    <author>tc={FEFDC51A-3490-4085-A8F8-72BFDA78A212}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{740B47BA-F5D4-4799-82B4-6217BAF24418}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     ID des Zeitabschnitts. Muss bei 0 beginnen und aufsteigen. Eine ID darf nicht doppelt vergeben werden.</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1" shapeId="0" xr:uid="{99CDC6AA-F96E-4729-8D1D-2E4CD2479760}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
-    Tag und Uhrzeit des Zeitabschnitts.</t>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Tag und Uhrzeit des Zeitabschnitts. Beispiel: "Fr 08:00" oder "Sa 10:15".</t>
       </text>
     </comment>
     <comment ref="C1" authorId="2" shapeId="0" xr:uid="{BEA58940-8B8B-44F6-A1BC-72CF21AEA3A9}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Block des Zeitabschnitts. 1 für Freitag, 2 für Samstag.</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{FEFDC51A-3490-4085-A8F8-72BFDA78A212}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Priorität, nach der ein Zeitabschnitt nicht verwendet werden soll. Höhere Zahl = Timeslot wird eher freigehalten.</t>
       </text>
     </comment>
   </commentList>
@@ -61,9 +70,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>datum</t>
-  </si>
-  <si>
     <t>block</t>
   </si>
   <si>
@@ -176,19 +182,28 @@
   </si>
   <si>
     <t>priority</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -215,7 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -233,6 +248,7 @@
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Peer Juettner" id="{C4787F05-2C8A-46A1-9CEC-39C1994241E4}" userId="Peer Juettner" providerId="None"/>
+  <person displayName="Peer Jüttner" id="{DE6415F7-933E-4839-9354-D53EFA2DC2FD}" userId="db361b8301d82d0a" providerId="Windows Live"/>
 </personList>
 </file>
 
@@ -562,10 +578,13 @@
     <text>ID des Zeitabschnitts. Muss bei 0 beginnen und aufsteigen. Eine ID darf nicht doppelt vergeben werden.</text>
   </threadedComment>
   <threadedComment ref="B1" dT="2020-03-21T13:34:13.35" personId="{C4787F05-2C8A-46A1-9CEC-39C1994241E4}" id="{99CDC6AA-F96E-4729-8D1D-2E4CD2479760}">
-    <text>Tag und Uhrzeit des Zeitabschnitts.</text>
+    <text>Tag und Uhrzeit des Zeitabschnitts. Beispiel: "Fr 08:00" oder "Sa 10:15".</text>
   </threadedComment>
   <threadedComment ref="C1" dT="2020-03-21T13:34:32.72" personId="{C4787F05-2C8A-46A1-9CEC-39C1994241E4}" id="{BEA58940-8B8B-44F6-A1BC-72CF21AEA3A9}">
     <text>Block des Zeitabschnitts. 1 für Freitag, 2 für Samstag.</text>
+  </threadedComment>
+  <threadedComment ref="D1" dT="2020-03-29T14:45:48.49" personId="{DE6415F7-933E-4839-9354-D53EFA2DC2FD}" id="{FEFDC51A-3490-4085-A8F8-72BFDA78A212}">
+    <text>Priorität, nach der ein Zeitabschnitt nicht verwendet werden soll. Höhere Zahl = Timeslot wird eher freigehalten.</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -575,272 +594,272 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D19">
         <v>5</v>
@@ -849,7 +868,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C1 A20:D21 A6:C6 A7:C7 A8:C8 A9:C9 A10:C10 A11:C11 A12:C12 A13:C13 A14:C14 A5:C5 A4:C4 A3:C3 A2:C2 A15:C15 A16:C16 A17:C17 A18:C18 A19:C19" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 A20:D21 A6:C6 A7:C7 A8:C8 A9:C9 A10:C10 A11:C11 A12:C12 A13:C13 A14:C14 A5:C5 A4:C4 A3:C3 A2:C2 A15:C15 A16:C16 A17:C17 A18:C18 A19:C19 C1" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>